<commit_message>
Working on processModifiedStudentsData() - processing making changes in studentsDict to a modified student
- also defined getStudentProcessedCourses()
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl-no-extra-requests-testing/Students-1.xlsx
+++ b/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl-no-extra-requests-testing/Students-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\2020-Sem1-CAES-Wvl-no-extra-requests-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60586F94-9648-4025-807A-36E15E49C561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B3E6F2-D81B-4F2C-A762-CCF0CF958634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="60" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="256">
   <si>
     <t>studentNumber</t>
   </si>
@@ -1125,7 +1125,7 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+      <selection activeCell="J99" sqref="J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4565,10 +4565,10 @@
       </c>
       <c r="G99" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H99" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="I99" t="s">
         <v>234</v>
@@ -4578,6 +4578,9 @@
       </c>
       <c r="K99" t="s">
         <v>225</v>
+      </c>
+      <c r="L99" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>